<commit_message>
budget working on all Qs! except still very slow.
</commit_message>
<xml_diff>
--- a/data/1038-0610-0614-day-larger-figures-test.xlsx
+++ b/data/1038-0610-0614-day-larger-figures-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{72E707BE-0160-4B47-9423-3E839962E439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EAF0E6C-2112-4DF4-9AF5-7B10343F1EEF}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{72E707BE-0160-4B47-9423-3E839962E439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{519346DE-E259-4608-AFAF-B4A35B4CF130}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="510" yWindow="4890" windowWidth="17670" windowHeight="9840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="675" windowWidth="18825" windowHeight="8235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AV5" sqref="AV5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,7 +1794,7 @@
         <v>89.690228174603106</v>
       </c>
       <c r="L7" s="20">
-        <v>79.132013670350801</v>
+        <v>89.132013670350801</v>
       </c>
       <c r="M7" s="20">
         <v>1</v>
@@ -2278,7 +2278,7 @@
         <v>9</v>
       </c>
       <c r="AT9" s="20">
-        <v>1.00461538461538</v>
+        <v>71.004615384615306</v>
       </c>
       <c r="AU9" s="20">
         <v>0</v>

</xml_diff>

<commit_message>
last test with smaller figures + working: works with Q2 on second run. others OK.
</commit_message>
<xml_diff>
--- a/data/1038-0610-0614-day-larger-figures-test.xlsx
+++ b/data/1038-0610-0614-day-larger-figures-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{72E707BE-0160-4B47-9423-3E839962E439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{519346DE-E259-4608-AFAF-B4A35B4CF130}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{72E707BE-0160-4B47-9423-3E839962E439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A83EA49F-FD48-4F55-B28D-B1775F13EF54}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="675" windowWidth="18825" windowHeight="8235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="3390" windowWidth="18825" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AV5" sqref="AV5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1888,7 @@
         <v>3</v>
       </c>
       <c r="AT7" s="20">
-        <v>17.543209999999998</v>
+        <v>13.54321</v>
       </c>
       <c r="AU7" s="20">
         <v>0</v>

</xml_diff>